<commit_message>
Updates/revisons to trans/BESP, trans/BMRESP, and trans/BPoEFUbVT
</commit_message>
<xml_diff>
--- a/InputData/trans/BMRESP/BAU Min Req EV Sales Perc.xlsx
+++ b/InputData/trans/BMRESP/BAU Min Req EV Sales Perc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\Documents\Energy Policy Simulator\California\3.0 Update\Data Sources\trans\BMRESP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\Documents\Energy Policy Simulator\Models\US States\eps-california\InputData\trans\BMRESP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EFC2DD-F07C-49B4-BFD8-F06195C85B66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8EC833-FEC9-4D23-B0C4-6CF9DE5E343F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3270" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39315" yWindow="4890" windowWidth="15330" windowHeight="16260" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,16 @@
     <sheet name="LDV frt sales weighting" sheetId="5" r:id="rId5"/>
     <sheet name="Advance Clean Trucks schedule" sheetId="6" r:id="rId6"/>
     <sheet name="HDV psg" sheetId="7" r:id="rId7"/>
+    <sheet name="EMFAC" sheetId="9" r:id="rId8"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
   <definedNames>
     <definedName name="cpi_2010to2012" localSheetId="5">#REF!</definedName>
+    <definedName name="cpi_2010to2012" localSheetId="7">#REF!</definedName>
     <definedName name="cpi_2010to2012">#REF!</definedName>
+    <definedName name="cpi_2013to2012" localSheetId="7">#REF!</definedName>
     <definedName name="cpi_2013to2012">#REF!</definedName>
     <definedName name="cpi_2014to2012">#REF!</definedName>
     <definedName name="cpi_2016to2012">#REF!</definedName>
@@ -44,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="169">
   <si>
     <t>BMRESP BAU Minimum Required EV Sales Percentage</t>
   </si>
@@ -406,9 +412,6 @@
     <t>Transit requirement approximated using large agency column</t>
   </si>
   <si>
-    <t>Assume transit covers half of HDV-psg vehicle sales (adjustment factor)</t>
-  </si>
-  <si>
     <t>MDVs</t>
   </si>
   <si>
@@ -437,6 +440,123 @@
   </si>
   <si>
     <t>Sales-weighted shares schedule</t>
+  </si>
+  <si>
+    <t>Calculated transit bus ratio</t>
+  </si>
+  <si>
+    <t>"Urban"</t>
+  </si>
+  <si>
+    <t>Statewide</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>BT</t>
+  </si>
+  <si>
+    <t>"School"</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>"All other buses"</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Vehicle Description</t>
+  </si>
+  <si>
+    <t>Share</t>
+  </si>
+  <si>
+    <t>Vehicle Population</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>GVWR Class</t>
+  </si>
+  <si>
+    <t>Vehicle Category</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Aggregate</t>
+  </si>
+  <si>
+    <t>Vehicle Population Output Aggregation</t>
+  </si>
+  <si>
+    <t>Number of Vehicles Registered at the Same Address</t>
+  </si>
+  <si>
+    <t>Model Year</t>
+  </si>
+  <si>
+    <t>Electric Mile Range</t>
+  </si>
+  <si>
+    <t>Fuel Technology</t>
+  </si>
+  <si>
+    <t>Fuel Type</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>GVWR Class output</t>
+  </si>
+  <si>
+    <t>B, All other buses</t>
+  </si>
+  <si>
+    <t>BT, Urban buses</t>
+  </si>
+  <si>
+    <t>BS, School buses</t>
+  </si>
+  <si>
+    <t>Calendar Year</t>
+  </si>
+  <si>
+    <t>statewide</t>
+  </si>
+  <si>
+    <t>Region type</t>
+  </si>
+  <si>
+    <t>Database query filters:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: The state government's EMFAC fleet database provides the basis for the ratio of transit buses vs school and other buses. </t>
+  </si>
+  <si>
+    <t>https://arb.ca.gov/emfac/fleet-db</t>
+  </si>
+  <si>
+    <t>Source: CARB Fleet Web Database</t>
+  </si>
+  <si>
+    <t>Class 4-8 vocational</t>
+  </si>
+  <si>
+    <t>Class 4-8 vocational ACT schedule</t>
+  </si>
+  <si>
+    <t>Fraction transit buses</t>
+  </si>
+  <si>
+    <t>Fraction non-transit buses</t>
   </si>
 </sst>
 </file>
@@ -553,7 +673,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,6 +701,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,7 +964,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -879,15 +1011,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="105" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -956,6 +1079,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="105" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="106">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1221,6 +1362,33 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="About"/>
+      <sheetName val="ZEV Waiver States"/>
+      <sheetName val="BMRESP-passenger"/>
+      <sheetName val="BMRESP-freight"/>
+      <sheetName val="Advance Clean Trucks schedule"/>
+      <sheetName val="LDV frt sales"/>
+      <sheetName val="HDV psg"/>
+      <sheetName val="EMFAC"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1546,7 +1714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -1640,12 +1808,12 @@
       </c>
     </row>
     <row r="20" spans="1:2" s="2" customFormat="1">
-      <c r="B20" s="44" t="s">
-        <v>125</v>
+      <c r="B20" s="41" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="2" customFormat="1">
-      <c r="B21" s="44"/>
+      <c r="B21" s="41"/>
     </row>
     <row r="22" spans="1:2" s="2" customFormat="1">
       <c r="B22" s="2" t="s">
@@ -1668,12 +1836,12 @@
       </c>
     </row>
     <row r="26" spans="1:2" s="2" customFormat="1">
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="41" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="2" customFormat="1">
-      <c r="B27" s="44"/>
+      <c r="B27" s="41"/>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
@@ -2552,7 +2720,7 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
@@ -2837,116 +3005,116 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <f>'HDV psg'!B17</f>
-        <v>0.125</v>
+        <f>'HDV psg'!B23</f>
+        <v>7.6549485831278213E-2</v>
       </c>
       <c r="J3">
-        <f>'HDV psg'!C17</f>
-        <v>0.125</v>
+        <f>'HDV psg'!C23</f>
+        <v>0.13899167093201806</v>
       </c>
       <c r="K3">
-        <f>'HDV psg'!D17</f>
-        <v>0.125</v>
+        <f>'HDV psg'!D23</f>
+        <v>0.1528677120655158</v>
       </c>
       <c r="L3">
-        <f>'HDV psg'!E17</f>
-        <v>0.25</v>
+        <f>'HDV psg'!E23</f>
+        <v>0.24329323903029176</v>
       </c>
       <c r="M3">
-        <f>'HDV psg'!F17</f>
-        <v>0.25</v>
+        <f>'HDV psg'!F23</f>
+        <v>0.29185938299753389</v>
       </c>
       <c r="N3">
-        <f>'HDV psg'!G17</f>
-        <v>0.25</v>
+        <f>'HDV psg'!G23</f>
+        <v>0.36123958866502259</v>
       </c>
       <c r="O3">
-        <f>'HDV psg'!H17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!H23</f>
+        <v>0.58371876599506778</v>
       </c>
       <c r="P3">
-        <f>'HDV psg'!I17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!I23</f>
+        <v>0.65309897166255637</v>
       </c>
       <c r="Q3">
-        <f>'HDV psg'!J17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!J23</f>
+        <v>0.68778907449630089</v>
       </c>
       <c r="R3">
-        <f>'HDV psg'!K17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!K23</f>
+        <v>0.72247917733004519</v>
       </c>
       <c r="S3">
-        <f>'HDV psg'!L17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!L23</f>
+        <v>0.75716928016378948</v>
       </c>
       <c r="T3">
-        <f>'HDV psg'!M17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!M23</f>
+        <v>0.79185938299753378</v>
       </c>
       <c r="U3">
-        <f>'HDV psg'!N17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!N23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="V3">
-        <f>'HDV psg'!O17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!O23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="W3">
-        <f>'HDV psg'!P17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!P23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="X3">
-        <f>'HDV psg'!Q17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!Q23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="Y3">
-        <f>'HDV psg'!R17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!R23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="Z3">
-        <f>'HDV psg'!S17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!S23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="AA3">
-        <f>'HDV psg'!T17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!T23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="AB3">
-        <f>'HDV psg'!U17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!U23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="AC3">
-        <f>'HDV psg'!V17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!V23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="AD3">
-        <f>'HDV psg'!W17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!W23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="AE3">
-        <f>'HDV psg'!X17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!X23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="AF3">
-        <f>'HDV psg'!Y17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!Y23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="AG3">
-        <f>'HDV psg'!Z17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!Z23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="AH3">
-        <f>'HDV psg'!AA17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!AA23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="AI3">
-        <f>'HDV psg'!AB17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!AB23</f>
+        <v>0.82654948583127819</v>
       </c>
       <c r="AJ3">
-        <f>'HDV psg'!AC17</f>
-        <v>0.5</v>
+        <f>'HDV psg'!AC23</f>
+        <v>0.82654948583127819</v>
       </c>
     </row>
     <row r="4" spans="1:36">
@@ -3401,7 +3569,7 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
@@ -4294,20 +4462,20 @@
       <c r="H17" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="J17" s="22" t="s">
+      <c r="J17" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="24"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="54"/>
       <c r="O17" s="12"/>
-      <c r="P17" s="22" t="s">
+      <c r="P17" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="24"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="53"/>
+      <c r="S17" s="54"/>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="13">
@@ -4349,7 +4517,7 @@
       <c r="M18" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="N18" s="25" t="s">
+      <c r="N18" s="22" t="s">
         <v>107</v>
       </c>
       <c r="O18" s="12"/>
@@ -4362,7 +4530,7 @@
       <c r="R18" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="S18" s="25" t="s">
+      <c r="S18" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4394,40 +4562,40 @@
         <f t="shared" ref="H19:H24" si="2">SUM(B19:E19)</f>
         <v>69552</v>
       </c>
-      <c r="J19" s="26">
+      <c r="J19" s="23">
         <f>B18/$G$18</f>
         <v>0.7308654395171158</v>
       </c>
-      <c r="K19" s="27">
+      <c r="K19" s="24">
         <f>C18/$G$18</f>
         <v>8.7495581717828105E-2</v>
       </c>
-      <c r="L19" s="27">
+      <c r="L19" s="24">
         <f>D18/$G$18</f>
         <v>0.10272166181788521</v>
       </c>
-      <c r="M19" s="27">
+      <c r="M19" s="24">
         <f>E18/$G$18</f>
         <v>1.5212485385682047E-2</v>
       </c>
-      <c r="N19" s="28">
+      <c r="N19" s="25">
         <f>F18/$G$18</f>
         <v>6.3704831561488887E-2</v>
       </c>
       <c r="O19" s="12"/>
-      <c r="P19" s="26">
+      <c r="P19" s="23">
         <f>B18/$H$18</f>
         <v>0.78059298408642119</v>
       </c>
-      <c r="Q19" s="27">
+      <c r="Q19" s="24">
         <f>C18/$H$18</f>
         <v>9.3448716459519104E-2</v>
       </c>
-      <c r="R19" s="27">
+      <c r="R19" s="24">
         <f>D18/$H$18</f>
         <v>0.10971076780113834</v>
       </c>
-      <c r="S19" s="28">
+      <c r="S19" s="25">
         <f>E18/$H$18</f>
         <v>1.6247531652921362E-2</v>
       </c>
@@ -4460,40 +4628,40 @@
         <f t="shared" si="2"/>
         <v>70385</v>
       </c>
-      <c r="J20" s="26">
+      <c r="J20" s="23">
         <f>B19/$G$19</f>
         <v>0.72949771935253827</v>
       </c>
-      <c r="K20" s="27">
+      <c r="K20" s="24">
         <f>C19/$G$19</f>
         <v>8.7875566798078605E-2</v>
       </c>
-      <c r="L20" s="27">
+      <c r="L20" s="24">
         <f>D19/$G$19</f>
         <v>0.10316061409292125</v>
       </c>
-      <c r="M20" s="27">
+      <c r="M20" s="24">
         <f>E19/$G$19</f>
         <v>1.529850244210923E-2</v>
       </c>
-      <c r="N20" s="28">
+      <c r="N20" s="25">
         <f>F19/$G$19</f>
         <v>6.4167597314352606E-2</v>
       </c>
       <c r="O20" s="12"/>
-      <c r="P20" s="26">
+      <c r="P20" s="23">
         <f>B19/$H$19</f>
         <v>0.77951748332183113</v>
       </c>
-      <c r="Q20" s="27">
+      <c r="Q20" s="24">
         <f>C19/$H$19</f>
         <v>9.390096618357488E-2</v>
       </c>
-      <c r="R20" s="27">
+      <c r="R20" s="24">
         <f>D19/$H$19</f>
         <v>0.11023406947319991</v>
       </c>
-      <c r="S20" s="28">
+      <c r="S20" s="25">
         <f>E19/$H$19</f>
         <v>1.6347481021394064E-2</v>
       </c>
@@ -4526,40 +4694,40 @@
         <f t="shared" si="2"/>
         <v>71098</v>
       </c>
-      <c r="J21" s="26">
+      <c r="J21" s="23">
         <f>B20/$G$20</f>
         <v>0.72710250587625991</v>
       </c>
-      <c r="K21" s="27">
+      <c r="K21" s="24">
         <f>C20/$G$20</f>
         <v>8.829661500869819E-2</v>
       </c>
-      <c r="L21" s="27">
+      <c r="L21" s="24">
         <f>D20/$G$20</f>
         <v>0.10366120871678419</v>
       </c>
-      <c r="M21" s="27">
+      <c r="M21" s="24">
         <f>E20/$G$20</f>
         <v>1.5630187376332948E-2</v>
       </c>
-      <c r="N21" s="28">
+      <c r="N21" s="25">
         <f>F20/$G$20</f>
         <v>6.5309483021924755E-2</v>
       </c>
       <c r="O21" s="12"/>
-      <c r="P21" s="26">
+      <c r="P21" s="23">
         <f>B20/$H$20</f>
         <v>0.77790722455068551</v>
       </c>
-      <c r="Q21" s="27">
+      <c r="Q21" s="24">
         <f>C20/$H$20</f>
         <v>9.4466150458194217E-2</v>
       </c>
-      <c r="R21" s="27">
+      <c r="R21" s="24">
         <f>D20/$H$20</f>
         <v>0.11090431199829509</v>
       </c>
-      <c r="S21" s="28">
+      <c r="S21" s="25">
         <f>E20/$H$20</f>
         <v>1.6722312992825176E-2</v>
       </c>
@@ -4592,40 +4760,40 @@
         <f t="shared" si="2"/>
         <v>71990</v>
       </c>
-      <c r="J22" s="26">
+      <c r="J22" s="23">
         <f>B21/$G$21</f>
         <v>0.72481633833173442</v>
       </c>
-      <c r="K22" s="27">
+      <c r="K22" s="24">
         <f>C21/$G$21</f>
         <v>8.9182689148519539E-2</v>
       </c>
-      <c r="L22" s="27">
+      <c r="L22" s="24">
         <f>D21/$G$21</f>
         <v>0.10469043645109145</v>
       </c>
-      <c r="M22" s="27">
+      <c r="M22" s="24">
         <f>E21/$G$21</f>
         <v>1.5691737524805825E-2</v>
       </c>
-      <c r="N22" s="28">
+      <c r="N22" s="25">
         <f>F21/$G$21</f>
         <v>6.5618798543848819E-2</v>
       </c>
       <c r="O22" s="12"/>
-      <c r="P22" s="26">
+      <c r="P22" s="23">
         <f>B21/$H$21</f>
         <v>0.77571802301049253</v>
       </c>
-      <c r="Q22" s="27">
+      <c r="Q22" s="24">
         <f>C21/$H$21</f>
         <v>9.54457228051422E-2</v>
       </c>
-      <c r="R22" s="27">
+      <c r="R22" s="24">
         <f>D21/$H$21</f>
         <v>0.11204253284199274</v>
       </c>
-      <c r="S22" s="28">
+      <c r="S22" s="25">
         <f>E21/$H$21</f>
         <v>1.6793721342372499E-2</v>
       </c>
@@ -4658,40 +4826,40 @@
         <f t="shared" si="2"/>
         <v>72880</v>
       </c>
-      <c r="J23" s="26">
+      <c r="J23" s="23">
         <f>B22/$G$22</f>
         <v>0.72360993966132481</v>
       </c>
-      <c r="K23" s="27">
+      <c r="K23" s="24">
         <f>C22/$G$22</f>
         <v>8.9586712515409075E-2</v>
       </c>
-      <c r="L23" s="27">
+      <c r="L23" s="24">
         <f>D22/$G$22</f>
         <v>0.10517095957957569</v>
       </c>
-      <c r="M23" s="27">
+      <c r="M23" s="24">
         <f>E22/$G$22</f>
         <v>1.5778887951729059E-2</v>
       </c>
-      <c r="N23" s="28">
+      <c r="N23" s="25">
         <f>F22/$G$22</f>
         <v>6.5853500291961325E-2</v>
       </c>
       <c r="O23" s="12"/>
-      <c r="P23" s="26">
+      <c r="P23" s="23">
         <f>B22/$H$22</f>
         <v>0.77462147520488955</v>
       </c>
-      <c r="Q23" s="27">
+      <c r="Q23" s="24">
         <f>C22/$H$22</f>
         <v>9.5902208640088901E-2</v>
       </c>
-      <c r="R23" s="27">
+      <c r="R23" s="24">
         <f>D22/$H$22</f>
         <v>0.11258508126128629</v>
       </c>
-      <c r="S23" s="28">
+      <c r="S23" s="25">
         <f>E22/$H$22</f>
         <v>1.689123489373524E-2</v>
       </c>
@@ -4723,40 +4891,40 @@
         <f t="shared" si="2"/>
         <v>73769</v>
       </c>
-      <c r="J24" s="26">
+      <c r="J24" s="23">
         <f>B23/$G$23</f>
         <v>0.72232544431773038</v>
       </c>
-      <c r="K24" s="27">
+      <c r="K24" s="24">
         <f>C23/$G$23</f>
         <v>9.0003972270985763E-2</v>
       </c>
-      <c r="L24" s="27">
+      <c r="L24" s="24">
         <f>D23/$G$23</f>
         <v>0.10566240822131956</v>
       </c>
-      <c r="M24" s="27">
+      <c r="M24" s="24">
         <f>E23/$G$23</f>
         <v>1.5876270165682143E-2</v>
       </c>
-      <c r="N24" s="28">
+      <c r="N24" s="25">
         <f>F23/$G$23</f>
         <v>6.6131905024282109E-2</v>
       </c>
       <c r="O24" s="12"/>
-      <c r="P24" s="26">
+      <c r="P24" s="23">
         <f>B23/$H$23</f>
         <v>0.77347694840834247</v>
       </c>
-      <c r="Q24" s="27">
+      <c r="Q24" s="24">
         <f>C23/$H$23</f>
         <v>9.6377607025246975E-2</v>
       </c>
-      <c r="R24" s="27">
+      <c r="R24" s="24">
         <f>D23/$H$23</f>
         <v>0.11314489571899013</v>
       </c>
-      <c r="S24" s="28">
+      <c r="S24" s="25">
         <f>E23/$H$23</f>
         <v>1.7000548847420416E-2</v>
       </c>
@@ -4766,151 +4934,151 @@
         <v>110</v>
       </c>
       <c r="B25" s="17">
-        <f>SUM(B18:B24)</f>
+        <f t="shared" ref="B25:H25" si="3">SUM(B18:B24)</f>
         <v>386987</v>
       </c>
       <c r="C25" s="17">
-        <f>SUM(C18:C24)</f>
+        <f t="shared" si="3"/>
         <v>47477</v>
       </c>
       <c r="D25" s="17">
-        <f>SUM(D18:D24)</f>
+        <f t="shared" si="3"/>
         <v>55736</v>
       </c>
       <c r="E25" s="17">
-        <f>SUM(E18:E24)</f>
+        <f t="shared" si="3"/>
         <v>8346</v>
       </c>
       <c r="F25" s="17">
-        <f>SUM(F18:F24)</f>
+        <f t="shared" si="3"/>
         <v>34865</v>
       </c>
       <c r="G25" s="18">
-        <f>SUM(G18:G24)</f>
+        <f t="shared" si="3"/>
         <v>533411</v>
       </c>
       <c r="H25" s="17">
-        <f>SUM(H18:H24)</f>
+        <f t="shared" si="3"/>
         <v>498546</v>
       </c>
-      <c r="J25" s="29">
+      <c r="J25" s="26">
         <f>B24/$G$24</f>
         <v>0.72082194554104662</v>
       </c>
-      <c r="K25" s="30">
+      <c r="K25" s="27">
         <f>C24/$G$24</f>
         <v>9.0431723858690152E-2</v>
       </c>
-      <c r="L25" s="30">
+      <c r="L25" s="27">
         <f>D24/$G$24</f>
         <v>0.10615953031683369</v>
       </c>
-      <c r="M25" s="30">
+      <c r="M25" s="27">
         <f>E24/$G$24</f>
         <v>1.599352161149914E-2</v>
       </c>
-      <c r="N25" s="31">
+      <c r="N25" s="28">
         <f>F24/$G$24</f>
         <v>6.659327867193035E-2</v>
       </c>
       <c r="O25" s="12"/>
-      <c r="P25" s="29">
+      <c r="P25" s="26">
         <f>B24/$H$24</f>
         <v>0.7722485054697773</v>
       </c>
-      <c r="Q25" s="30">
+      <c r="Q25" s="27">
         <f>C24/$H$24</f>
         <v>9.6883514755520608E-2</v>
       </c>
-      <c r="R25" s="30">
+      <c r="R25" s="27">
         <f>D24/$H$24</f>
         <v>0.11373341105342352</v>
       </c>
-      <c r="S25" s="31">
+      <c r="S25" s="28">
         <f>E24/$H$24</f>
         <v>1.7134568721278585E-2</v>
       </c>
     </row>
     <row r="27" spans="1:19">
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="C27" s="33"/>
+      <c r="C27" s="30"/>
     </row>
     <row r="28" spans="1:19">
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="C28" s="35">
+      <c r="C28" s="32">
         <f>B25+C25+D25</f>
         <v>490200</v>
       </c>
     </row>
     <row r="29" spans="1:19">
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="C29" s="35">
+      <c r="C29" s="32">
         <f>B25+C25+D25+E25</f>
         <v>498546</v>
       </c>
     </row>
     <row r="30" spans="1:19">
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="38">
+      <c r="C30" s="35">
         <f>F25</f>
         <v>34865</v>
       </c>
     </row>
     <row r="32" spans="1:19">
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="33"/>
+      <c r="C32" s="30"/>
     </row>
     <row r="33" spans="2:3">
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="40">
+      <c r="C33" s="37">
         <f>B25/C29</f>
         <v>0.7762312805638798</v>
       </c>
     </row>
     <row r="34" spans="2:3">
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="40">
+      <c r="C34" s="37">
         <f>C25/C29</f>
         <v>9.5230931548944325E-2</v>
       </c>
     </row>
     <row r="35" spans="2:3">
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="40">
+      <c r="C35" s="37">
         <f>D25/C29</f>
         <v>0.11179710598420206</v>
       </c>
     </row>
     <row r="36" spans="2:3">
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="41">
+      <c r="C36" s="38">
         <f>E25/C29</f>
         <v>1.6740681902973849E-2</v>
       </c>
     </row>
     <row r="37" spans="2:3">
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="43">
+      <c r="C37" s="40">
         <f>SUM(C33:C36)</f>
         <v>1</v>
       </c>
@@ -4935,7 +5103,9 @@
   </sheetPr>
   <dimension ref="A1:AB89"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="14.25"/>
   <cols>
@@ -4955,7 +5125,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -4964,69 +5134,69 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="B20" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="22" t="s">
+      <c r="B20" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="M20" s="23"/>
-      <c r="N20" s="24"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="M20" s="53"/>
+      <c r="N20" s="54"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C21" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="46">
+      <c r="E21" s="43">
         <v>8</v>
       </c>
-      <c r="F21" s="47" t="s">
+      <c r="F21" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="G21" s="45" t="str">
+      <c r="G21" s="42" t="str">
         <f>'LDV frt sales weighting'!J18</f>
         <v>Class 2b-3</v>
       </c>
-      <c r="H21" s="46" t="str">
+      <c r="H21" s="43" t="str">
         <f>'LDV frt sales weighting'!K18</f>
         <v>Class 4-5</v>
       </c>
-      <c r="I21" s="46" t="str">
+      <c r="I21" s="43" t="str">
         <f>'LDV frt sales weighting'!L18</f>
         <v>Class 6-7</v>
       </c>
-      <c r="J21" s="46" t="str">
+      <c r="J21" s="43" t="str">
         <f>'LDV frt sales weighting'!M18</f>
         <v>Class 8</v>
       </c>
-      <c r="K21" s="47" t="str">
+      <c r="K21" s="44" t="str">
         <f>'LDV frt sales weighting'!N18</f>
         <v>Class 7-8 Tractor</v>
       </c>
       <c r="L21" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="M21" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="M21" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="N21" s="25" t="s">
+      <c r="N21" s="22" t="s">
         <v>70</v>
       </c>
     </row>
@@ -5035,51 +5205,51 @@
         <f>'LDV frt sales weighting'!A18</f>
         <v>2024</v>
       </c>
-      <c r="B22" s="48">
+      <c r="B22" s="45">
         <v>0.05</v>
       </c>
-      <c r="C22" s="49">
+      <c r="C22" s="46">
         <v>0.09</v>
       </c>
-      <c r="D22" s="49">
+      <c r="D22" s="46">
         <v>0.09</v>
       </c>
-      <c r="E22" s="49">
+      <c r="E22" s="46">
         <v>0.09</v>
       </c>
-      <c r="F22" s="50">
+      <c r="F22" s="47">
         <v>0.05</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G22" s="23">
         <f>'LDV frt sales weighting'!J19</f>
         <v>0.7308654395171158</v>
       </c>
-      <c r="H22" s="27">
+      <c r="H22" s="24">
         <f>'LDV frt sales weighting'!K19</f>
         <v>8.7495581717828105E-2</v>
       </c>
-      <c r="I22" s="27">
+      <c r="I22" s="24">
         <f>'LDV frt sales weighting'!L19</f>
         <v>0.10272166181788521</v>
       </c>
-      <c r="J22" s="27">
+      <c r="J22" s="24">
         <f>'LDV frt sales weighting'!M19</f>
         <v>1.5212485385682047E-2</v>
       </c>
-      <c r="K22" s="28">
+      <c r="K22" s="25">
         <f>'LDV frt sales weighting'!N19</f>
         <v>6.3704831561488887E-2</v>
       </c>
-      <c r="L22" s="26">
+      <c r="L22" s="23">
         <f>G22*B22+H22*C22+I22*D22+J22*E22</f>
         <v>5.5031947578781375E-2</v>
       </c>
-      <c r="M22" s="27">
+      <c r="M22" s="24">
         <f>G22*B22+H22*C22+I22*D22+J22*E22+K22*F22</f>
         <v>5.8217189156855823E-2</v>
       </c>
-      <c r="N22" s="28">
-        <f>F22</f>
+      <c r="N22" s="25">
+        <f t="shared" ref="N22:N33" si="0">F22</f>
         <v>0.05</v>
       </c>
     </row>
@@ -5088,51 +5258,51 @@
         <f>'LDV frt sales weighting'!A19</f>
         <v>2025</v>
       </c>
-      <c r="B23" s="48">
+      <c r="B23" s="45">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C23" s="49">
+      <c r="C23" s="46">
         <v>0.11</v>
       </c>
-      <c r="D23" s="49">
+      <c r="D23" s="46">
         <v>0.11</v>
       </c>
-      <c r="E23" s="49">
+      <c r="E23" s="46">
         <v>0.11</v>
       </c>
-      <c r="F23" s="50">
+      <c r="F23" s="47">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G23" s="26">
+      <c r="G23" s="23">
         <f>'LDV frt sales weighting'!J20</f>
         <v>0.72949771935253827</v>
       </c>
-      <c r="H23" s="27">
+      <c r="H23" s="24">
         <f>'LDV frt sales weighting'!K20</f>
         <v>8.7875566798078605E-2</v>
       </c>
-      <c r="I23" s="27">
+      <c r="I23" s="24">
         <f>'LDV frt sales weighting'!L20</f>
         <v>0.10316061409292125</v>
       </c>
-      <c r="J23" s="27">
+      <c r="J23" s="24">
         <f>'LDV frt sales weighting'!M20</f>
         <v>1.529850244210923E-2</v>
       </c>
-      <c r="K23" s="28">
+      <c r="K23" s="25">
         <f>'LDV frt sales weighting'!N20</f>
         <v>6.4167597314352606E-2</v>
       </c>
-      <c r="L23" s="26">
-        <f>G23*B23+H23*C23+I23*D23+J23*E23</f>
+      <c r="L23" s="23">
+        <f t="shared" ref="L22:L33" si="1">G23*B23+H23*C23+I23*D23+J23*E23</f>
         <v>7.3761655521319677E-2</v>
       </c>
-      <c r="M23" s="27">
-        <f>G23*B23+H23*C23+I23*D23+J23*E23+K23*F23</f>
+      <c r="M23" s="24">
+        <f t="shared" ref="M22:M33" si="2">G23*B23+H23*C23+I23*D23+J23*E23+K23*F23</f>
         <v>7.8253387333324362E-2</v>
       </c>
-      <c r="N23" s="28">
-        <f>F23</f>
+      <c r="N23" s="25">
+        <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -5141,51 +5311,51 @@
         <f>'LDV frt sales weighting'!A20</f>
         <v>2026</v>
       </c>
-      <c r="B24" s="48">
+      <c r="B24" s="45">
         <v>0.1</v>
       </c>
-      <c r="C24" s="49">
+      <c r="C24" s="46">
         <v>0.13</v>
       </c>
-      <c r="D24" s="49">
+      <c r="D24" s="46">
         <v>0.13</v>
       </c>
-      <c r="E24" s="49">
+      <c r="E24" s="46">
         <v>0.13</v>
       </c>
-      <c r="F24" s="50">
+      <c r="F24" s="47">
         <v>0.1</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="23">
         <f>'LDV frt sales weighting'!J21</f>
         <v>0.72710250587625991</v>
       </c>
-      <c r="H24" s="27">
+      <c r="H24" s="24">
         <f>'LDV frt sales weighting'!K21</f>
         <v>8.829661500869819E-2</v>
       </c>
-      <c r="I24" s="27">
+      <c r="I24" s="24">
         <f>'LDV frt sales weighting'!L21</f>
         <v>0.10366120871678419</v>
       </c>
-      <c r="J24" s="27">
+      <c r="J24" s="24">
         <f>'LDV frt sales weighting'!M21</f>
         <v>1.5630187376332948E-2</v>
       </c>
-      <c r="K24" s="28">
+      <c r="K24" s="25">
         <f>'LDV frt sales weighting'!N21</f>
         <v>6.5309483021924755E-2</v>
       </c>
-      <c r="L24" s="26">
-        <f>G24*B24+H24*C24+I24*D24+J24*E24</f>
+      <c r="L24" s="23">
+        <f t="shared" si="1"/>
         <v>9.9696692030861997E-2</v>
       </c>
-      <c r="M24" s="27">
-        <f>G24*B24+H24*C24+I24*D24+J24*E24+K24*F24</f>
+      <c r="M24" s="24">
+        <f t="shared" si="2"/>
         <v>0.10622764033305447</v>
       </c>
-      <c r="N24" s="28">
-        <f>F24</f>
+      <c r="N24" s="25">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
@@ -5194,51 +5364,51 @@
         <f>'LDV frt sales weighting'!A21</f>
         <v>2027</v>
       </c>
-      <c r="B25" s="48">
+      <c r="B25" s="45">
         <v>0.15</v>
       </c>
-      <c r="C25" s="49">
+      <c r="C25" s="46">
         <v>0.2</v>
       </c>
-      <c r="D25" s="49">
+      <c r="D25" s="46">
         <v>0.2</v>
       </c>
-      <c r="E25" s="49">
+      <c r="E25" s="46">
         <v>0.2</v>
       </c>
-      <c r="F25" s="50">
+      <c r="F25" s="47">
         <v>0.15</v>
       </c>
-      <c r="G25" s="26">
+      <c r="G25" s="23">
         <f>'LDV frt sales weighting'!J22</f>
         <v>0.72481633833173442</v>
       </c>
-      <c r="H25" s="27">
+      <c r="H25" s="24">
         <f>'LDV frt sales weighting'!K22</f>
         <v>8.9182689148519539E-2</v>
       </c>
-      <c r="I25" s="27">
+      <c r="I25" s="24">
         <f>'LDV frt sales weighting'!L22</f>
         <v>0.10469043645109145</v>
       </c>
-      <c r="J25" s="27">
+      <c r="J25" s="24">
         <f>'LDV frt sales weighting'!M22</f>
         <v>1.5691737524805825E-2</v>
       </c>
-      <c r="K25" s="28">
+      <c r="K25" s="25">
         <f>'LDV frt sales weighting'!N22</f>
         <v>6.5618798543848819E-2</v>
       </c>
-      <c r="L25" s="26">
-        <f>G25*B25+H25*C25+I25*D25+J25*E25</f>
+      <c r="L25" s="23">
+        <f t="shared" si="1"/>
         <v>0.15063542337464353</v>
       </c>
-      <c r="M25" s="27">
-        <f>G25*B25+H25*C25+I25*D25+J25*E25+K25*F25</f>
+      <c r="M25" s="24">
+        <f t="shared" si="2"/>
         <v>0.16047824315622086</v>
       </c>
-      <c r="N25" s="28">
-        <f>F25</f>
+      <c r="N25" s="25">
+        <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
     </row>
@@ -5247,51 +5417,51 @@
         <f>'LDV frt sales weighting'!A22</f>
         <v>2028</v>
       </c>
-      <c r="B26" s="48">
+      <c r="B26" s="45">
         <v>0.2</v>
       </c>
-      <c r="C26" s="49">
+      <c r="C26" s="46">
         <v>0.3</v>
       </c>
-      <c r="D26" s="49">
+      <c r="D26" s="46">
         <v>0.3</v>
       </c>
-      <c r="E26" s="49">
+      <c r="E26" s="46">
         <v>0.3</v>
       </c>
-      <c r="F26" s="50">
+      <c r="F26" s="47">
         <v>0.2</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="23">
         <f>'LDV frt sales weighting'!J23</f>
         <v>0.72360993966132481</v>
       </c>
-      <c r="H26" s="27">
+      <c r="H26" s="24">
         <f>'LDV frt sales weighting'!K23</f>
         <v>8.9586712515409075E-2</v>
       </c>
-      <c r="I26" s="27">
+      <c r="I26" s="24">
         <f>'LDV frt sales weighting'!L23</f>
         <v>0.10517095957957569</v>
       </c>
-      <c r="J26" s="27">
+      <c r="J26" s="24">
         <f>'LDV frt sales weighting'!M23</f>
         <v>1.5778887951729059E-2</v>
       </c>
-      <c r="K26" s="28">
+      <c r="K26" s="25">
         <f>'LDV frt sales weighting'!N23</f>
         <v>6.5853500291961325E-2</v>
       </c>
-      <c r="L26" s="26">
-        <f>G26*B26+H26*C26+I26*D26+J26*E26</f>
+      <c r="L26" s="23">
+        <f t="shared" si="1"/>
         <v>0.20788295594627912</v>
       </c>
-      <c r="M26" s="27">
-        <f>G26*B26+H26*C26+I26*D26+J26*E26+K26*F26</f>
+      <c r="M26" s="24">
+        <f t="shared" si="2"/>
         <v>0.22105365600467139</v>
       </c>
-      <c r="N26" s="28">
-        <f>F26</f>
+      <c r="N26" s="25">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -5300,51 +5470,51 @@
         <f>'LDV frt sales weighting'!A23</f>
         <v>2029</v>
       </c>
-      <c r="B27" s="48">
+      <c r="B27" s="45">
         <v>0.25</v>
       </c>
-      <c r="C27" s="49">
+      <c r="C27" s="46">
         <v>0.4</v>
       </c>
-      <c r="D27" s="49">
+      <c r="D27" s="46">
         <v>0.4</v>
       </c>
-      <c r="E27" s="49">
+      <c r="E27" s="46">
         <v>0.4</v>
       </c>
-      <c r="F27" s="50">
+      <c r="F27" s="47">
         <v>0.25</v>
       </c>
-      <c r="G27" s="26">
+      <c r="G27" s="23">
         <f>'LDV frt sales weighting'!J24</f>
         <v>0.72232544431773038</v>
       </c>
-      <c r="H27" s="27">
+      <c r="H27" s="24">
         <f>'LDV frt sales weighting'!K24</f>
         <v>9.0003972270985763E-2</v>
       </c>
-      <c r="I27" s="27">
+      <c r="I27" s="24">
         <f>'LDV frt sales weighting'!L24</f>
         <v>0.10566240822131956</v>
       </c>
-      <c r="J27" s="27">
+      <c r="J27" s="24">
         <f>'LDV frt sales weighting'!M24</f>
         <v>1.5876270165682143E-2</v>
       </c>
-      <c r="K27" s="28">
+      <c r="K27" s="25">
         <f>'LDV frt sales weighting'!N24</f>
         <v>6.6131905024282109E-2</v>
       </c>
-      <c r="L27" s="26">
-        <f>G27*B27+H27*C27+I27*D27+J27*E27</f>
+      <c r="L27" s="23">
+        <f t="shared" si="1"/>
         <v>0.26519842134262755</v>
       </c>
-      <c r="M27" s="27">
-        <f>G27*B27+H27*C27+I27*D27+J27*E27+K27*F27</f>
+      <c r="M27" s="24">
+        <f t="shared" si="2"/>
         <v>0.28173139759869809</v>
       </c>
-      <c r="N27" s="28">
-        <f>F27</f>
+      <c r="N27" s="25">
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
@@ -5353,51 +5523,51 @@
         <f>'LDV frt sales weighting'!A24</f>
         <v>2030</v>
       </c>
-      <c r="B28" s="48">
+      <c r="B28" s="45">
         <v>0.3</v>
       </c>
-      <c r="C28" s="49">
+      <c r="C28" s="46">
         <v>0.5</v>
       </c>
-      <c r="D28" s="49">
+      <c r="D28" s="46">
         <v>0.5</v>
       </c>
-      <c r="E28" s="49">
+      <c r="E28" s="46">
         <v>0.5</v>
       </c>
-      <c r="F28" s="50">
+      <c r="F28" s="47">
         <v>0.3</v>
       </c>
-      <c r="G28" s="26">
+      <c r="G28" s="23">
         <f>'LDV frt sales weighting'!J25</f>
         <v>0.72082194554104662</v>
       </c>
-      <c r="H28" s="27">
+      <c r="H28" s="24">
         <f>'LDV frt sales weighting'!K25</f>
         <v>9.0431723858690152E-2</v>
       </c>
-      <c r="I28" s="27">
+      <c r="I28" s="24">
         <f>'LDV frt sales weighting'!L25</f>
         <v>0.10615953031683369</v>
       </c>
-      <c r="J28" s="27">
+      <c r="J28" s="24">
         <f>'LDV frt sales weighting'!M25</f>
         <v>1.599352161149914E-2</v>
       </c>
-      <c r="K28" s="28">
+      <c r="K28" s="25">
         <f>'LDV frt sales weighting'!N25</f>
         <v>6.659327867193035E-2</v>
       </c>
-      <c r="L28" s="26">
-        <f>G28*B28+H28*C28+I28*D28+J28*E28</f>
+      <c r="L28" s="23">
+        <f t="shared" si="1"/>
         <v>0.32253897155582545</v>
       </c>
-      <c r="M28" s="27">
-        <f>G28*B28+H28*C28+I28*D28+J28*E28+K28*F28</f>
+      <c r="M28" s="24">
+        <f t="shared" si="2"/>
         <v>0.34251695515740455</v>
       </c>
-      <c r="N28" s="28">
-        <f>F28</f>
+      <c r="N28" s="25">
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
     </row>
@@ -5406,210 +5576,210 @@
         <f>A28+1</f>
         <v>2031</v>
       </c>
-      <c r="B29" s="48">
+      <c r="B29" s="45">
         <v>0.35</v>
       </c>
-      <c r="C29" s="49">
+      <c r="C29" s="46">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D29" s="49">
+      <c r="D29" s="46">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E29" s="49">
+      <c r="E29" s="46">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F29" s="50">
+      <c r="F29" s="47">
         <v>0.35</v>
       </c>
-      <c r="G29" s="26">
-        <f t="shared" ref="G29:K33" si="0">G28</f>
+      <c r="G29" s="23">
+        <f t="shared" ref="G29:K33" si="3">G28</f>
         <v>0.72082194554104662</v>
       </c>
-      <c r="H29" s="27">
-        <f t="shared" si="0"/>
+      <c r="H29" s="24">
+        <f t="shared" si="3"/>
         <v>9.0431723858690152E-2</v>
       </c>
-      <c r="I29" s="27">
-        <f t="shared" si="0"/>
+      <c r="I29" s="24">
+        <f t="shared" si="3"/>
         <v>0.10615953031683369</v>
       </c>
-      <c r="J29" s="27">
-        <f t="shared" si="0"/>
+      <c r="J29" s="24">
+        <f t="shared" si="3"/>
         <v>1.599352161149914E-2</v>
       </c>
-      <c r="K29" s="28">
-        <f t="shared" si="0"/>
+      <c r="K29" s="25">
+        <f t="shared" si="3"/>
         <v>6.659327867193035E-2</v>
       </c>
-      <c r="L29" s="26">
-        <f>G29*B29+H29*C29+I29*D29+J29*E29</f>
+      <c r="L29" s="23">
+        <f t="shared" si="1"/>
         <v>0.36920930762222898</v>
       </c>
-      <c r="M29" s="27">
-        <f>G29*B29+H29*C29+I29*D29+J29*E29+K29*F29</f>
+      <c r="M29" s="24">
+        <f t="shared" si="2"/>
         <v>0.39251695515740459</v>
       </c>
-      <c r="N29" s="28">
-        <f>F29</f>
+      <c r="N29" s="25">
+        <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="13">
-        <f t="shared" ref="A30:A32" si="1">A29+1</f>
+        <f t="shared" ref="A30:A32" si="4">A29+1</f>
         <v>2032</v>
       </c>
-      <c r="B30" s="48">
+      <c r="B30" s="45">
         <v>0.4</v>
       </c>
-      <c r="C30" s="49">
+      <c r="C30" s="46">
         <v>0.6</v>
       </c>
-      <c r="D30" s="49">
+      <c r="D30" s="46">
         <v>0.6</v>
       </c>
-      <c r="E30" s="49">
+      <c r="E30" s="46">
         <v>0.6</v>
       </c>
-      <c r="F30" s="50">
+      <c r="F30" s="47">
         <v>0.4</v>
       </c>
-      <c r="G30" s="26">
-        <f t="shared" si="0"/>
+      <c r="G30" s="23">
+        <f t="shared" si="3"/>
         <v>0.72082194554104662</v>
       </c>
-      <c r="H30" s="27">
-        <f t="shared" si="0"/>
+      <c r="H30" s="24">
+        <f t="shared" si="3"/>
         <v>9.0431723858690152E-2</v>
       </c>
-      <c r="I30" s="27">
-        <f t="shared" si="0"/>
+      <c r="I30" s="24">
+        <f t="shared" si="3"/>
         <v>0.10615953031683369</v>
       </c>
-      <c r="J30" s="27">
-        <f t="shared" si="0"/>
+      <c r="J30" s="24">
+        <f t="shared" si="3"/>
         <v>1.599352161149914E-2</v>
       </c>
-      <c r="K30" s="28">
-        <f t="shared" si="0"/>
+      <c r="K30" s="25">
+        <f t="shared" si="3"/>
         <v>6.659327867193035E-2</v>
       </c>
-      <c r="L30" s="26">
-        <f>G30*B30+H30*C30+I30*D30+J30*E30</f>
+      <c r="L30" s="23">
+        <f t="shared" si="1"/>
         <v>0.41587964368863245</v>
       </c>
-      <c r="M30" s="27">
-        <f>G30*B30+H30*C30+I30*D30+J30*E30+K30*F30</f>
+      <c r="M30" s="24">
+        <f t="shared" si="2"/>
         <v>0.44251695515740458</v>
       </c>
-      <c r="N30" s="28">
-        <f>F30</f>
+      <c r="N30" s="25">
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="13">
+        <f t="shared" si="4"/>
+        <v>2033</v>
+      </c>
+      <c r="B31" s="45">
+        <v>0.45</v>
+      </c>
+      <c r="C31" s="46">
+        <v>0.65</v>
+      </c>
+      <c r="D31" s="46">
+        <v>0.65</v>
+      </c>
+      <c r="E31" s="46">
+        <v>0.65</v>
+      </c>
+      <c r="F31" s="47">
+        <v>0.4</v>
+      </c>
+      <c r="G31" s="23">
+        <f t="shared" si="3"/>
+        <v>0.72082194554104662</v>
+      </c>
+      <c r="H31" s="24">
+        <f t="shared" si="3"/>
+        <v>9.0431723858690152E-2</v>
+      </c>
+      <c r="I31" s="24">
+        <f t="shared" si="3"/>
+        <v>0.10615953031683369</v>
+      </c>
+      <c r="J31" s="24">
+        <f t="shared" si="3"/>
+        <v>1.599352161149914E-2</v>
+      </c>
+      <c r="K31" s="25">
+        <f t="shared" si="3"/>
+        <v>6.659327867193035E-2</v>
+      </c>
+      <c r="L31" s="23">
         <f t="shared" si="1"/>
-        <v>2033</v>
-      </c>
-      <c r="B31" s="48">
-        <v>0.45</v>
-      </c>
-      <c r="C31" s="49">
-        <v>0.65</v>
-      </c>
-      <c r="D31" s="49">
-        <v>0.65</v>
-      </c>
-      <c r="E31" s="49">
-        <v>0.65</v>
-      </c>
-      <c r="F31" s="50">
-        <v>0.4</v>
-      </c>
-      <c r="G31" s="26">
-        <f t="shared" si="0"/>
-        <v>0.72082194554104662</v>
-      </c>
-      <c r="H31" s="27">
-        <f t="shared" si="0"/>
-        <v>9.0431723858690152E-2</v>
-      </c>
-      <c r="I31" s="27">
-        <f t="shared" si="0"/>
-        <v>0.10615953031683369</v>
-      </c>
-      <c r="J31" s="27">
-        <f t="shared" si="0"/>
-        <v>1.599352161149914E-2</v>
-      </c>
-      <c r="K31" s="28">
-        <f t="shared" si="0"/>
-        <v>6.659327867193035E-2</v>
-      </c>
-      <c r="L31" s="26">
-        <f>G31*B31+H31*C31+I31*D31+J31*E31</f>
         <v>0.46254997975503592</v>
       </c>
-      <c r="M31" s="27">
-        <f>G31*B31+H31*C31+I31*D31+J31*E31+K31*F31</f>
+      <c r="M31" s="24">
+        <f t="shared" si="2"/>
         <v>0.48918729122380805</v>
       </c>
-      <c r="N31" s="28">
-        <f>F31</f>
+      <c r="N31" s="25">
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="13">
+        <f t="shared" si="4"/>
+        <v>2034</v>
+      </c>
+      <c r="B32" s="45">
+        <v>0.5</v>
+      </c>
+      <c r="C32" s="46">
+        <v>0.7</v>
+      </c>
+      <c r="D32" s="46">
+        <v>0.7</v>
+      </c>
+      <c r="E32" s="46">
+        <v>0.7</v>
+      </c>
+      <c r="F32" s="47">
+        <v>0.4</v>
+      </c>
+      <c r="G32" s="23">
+        <f t="shared" si="3"/>
+        <v>0.72082194554104662</v>
+      </c>
+      <c r="H32" s="24">
+        <f t="shared" si="3"/>
+        <v>9.0431723858690152E-2</v>
+      </c>
+      <c r="I32" s="24">
+        <f t="shared" si="3"/>
+        <v>0.10615953031683369</v>
+      </c>
+      <c r="J32" s="24">
+        <f t="shared" si="3"/>
+        <v>1.599352161149914E-2</v>
+      </c>
+      <c r="K32" s="25">
+        <f t="shared" si="3"/>
+        <v>6.659327867193035E-2</v>
+      </c>
+      <c r="L32" s="23">
         <f t="shared" si="1"/>
-        <v>2034</v>
-      </c>
-      <c r="B32" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="C32" s="49">
-        <v>0.7</v>
-      </c>
-      <c r="D32" s="49">
-        <v>0.7</v>
-      </c>
-      <c r="E32" s="49">
-        <v>0.7</v>
-      </c>
-      <c r="F32" s="50">
-        <v>0.4</v>
-      </c>
-      <c r="G32" s="26">
-        <f t="shared" si="0"/>
-        <v>0.72082194554104662</v>
-      </c>
-      <c r="H32" s="27">
-        <f t="shared" si="0"/>
-        <v>9.0431723858690152E-2</v>
-      </c>
-      <c r="I32" s="27">
-        <f t="shared" si="0"/>
-        <v>0.10615953031683369</v>
-      </c>
-      <c r="J32" s="27">
-        <f t="shared" si="0"/>
-        <v>1.599352161149914E-2</v>
-      </c>
-      <c r="K32" s="28">
-        <f t="shared" si="0"/>
-        <v>6.659327867193035E-2</v>
-      </c>
-      <c r="L32" s="26">
-        <f>G32*B32+H32*C32+I32*D32+J32*E32</f>
         <v>0.50922031582143934</v>
       </c>
-      <c r="M32" s="27">
-        <f>G32*B32+H32*C32+I32*D32+J32*E32+K32*F32</f>
+      <c r="M32" s="24">
+        <f t="shared" si="2"/>
         <v>0.53585762729021147</v>
       </c>
-      <c r="N32" s="28">
-        <f>F32</f>
+      <c r="N32" s="25">
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
@@ -5618,85 +5788,85 @@
         <f>A32+1</f>
         <v>2035</v>
       </c>
-      <c r="B33" s="51">
+      <c r="B33" s="48">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C33" s="52">
+      <c r="C33" s="49">
         <v>0.75</v>
       </c>
-      <c r="D33" s="52">
+      <c r="D33" s="49">
         <v>0.75</v>
       </c>
-      <c r="E33" s="52">
+      <c r="E33" s="49">
         <v>0.75</v>
       </c>
-      <c r="F33" s="53">
+      <c r="F33" s="50">
         <v>0.4</v>
       </c>
-      <c r="G33" s="29">
-        <f t="shared" si="0"/>
+      <c r="G33" s="26">
+        <f t="shared" si="3"/>
         <v>0.72082194554104662</v>
       </c>
-      <c r="H33" s="30">
-        <f t="shared" si="0"/>
+      <c r="H33" s="27">
+        <f t="shared" si="3"/>
         <v>9.0431723858690152E-2</v>
       </c>
-      <c r="I33" s="30">
-        <f t="shared" si="0"/>
+      <c r="I33" s="27">
+        <f t="shared" si="3"/>
         <v>0.10615953031683369</v>
       </c>
-      <c r="J33" s="30">
-        <f t="shared" si="0"/>
+      <c r="J33" s="27">
+        <f t="shared" si="3"/>
         <v>1.599352161149914E-2</v>
       </c>
-      <c r="K33" s="31">
-        <f t="shared" si="0"/>
+      <c r="K33" s="28">
+        <f t="shared" si="3"/>
         <v>6.659327867193035E-2</v>
       </c>
-      <c r="L33" s="29">
-        <f>G33*B33+H33*C33+I33*D33+J33*E33</f>
+      <c r="L33" s="26">
+        <f t="shared" si="1"/>
         <v>0.55589065188784292</v>
       </c>
-      <c r="M33" s="30">
-        <f>G33*B33+H33*C33+I33*D33+J33*E33+K33*F33</f>
+      <c r="M33" s="27">
+        <f t="shared" si="2"/>
         <v>0.58252796335661505</v>
       </c>
-      <c r="N33" s="31">
-        <f>F33</f>
+      <c r="N33" s="28">
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="36" spans="1:28">
       <c r="A36" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B36" s="54"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="54"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="54"/>
-      <c r="M36" s="54"/>
-      <c r="N36" s="54"/>
-      <c r="O36" s="54"/>
-      <c r="P36" s="54"/>
-      <c r="Q36" s="54"/>
-      <c r="R36" s="54"/>
-      <c r="S36" s="54"/>
-      <c r="T36" s="54"/>
-      <c r="U36" s="54"/>
-      <c r="V36" s="54"/>
-      <c r="W36" s="54"/>
-      <c r="X36" s="54"/>
-      <c r="Y36" s="54"/>
-      <c r="Z36" s="54"/>
-      <c r="AA36" s="54"/>
-      <c r="AB36" s="54"/>
+        <v>129</v>
+      </c>
+      <c r="B36" s="51"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="51"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="51"/>
+      <c r="O36" s="51"/>
+      <c r="P36" s="51"/>
+      <c r="Q36" s="51"/>
+      <c r="R36" s="51"/>
+      <c r="S36" s="51"/>
+      <c r="T36" s="51"/>
+      <c r="U36" s="51"/>
+      <c r="V36" s="51"/>
+      <c r="W36" s="51"/>
+      <c r="X36" s="51"/>
+      <c r="Y36" s="51"/>
+      <c r="Z36" s="51"/>
+      <c r="AA36" s="51"/>
+      <c r="AB36" s="51"/>
     </row>
     <row r="37" spans="1:28">
       <c r="B37" s="13">
@@ -5740,31 +5910,31 @@
         <v>2036</v>
       </c>
       <c r="O37" s="13">
-        <f t="shared" ref="O37:U37" si="2">N37+1</f>
+        <f t="shared" ref="O37:U37" si="5">N37+1</f>
         <v>2037</v>
       </c>
       <c r="P37" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2038</v>
       </c>
       <c r="Q37" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2039</v>
       </c>
       <c r="R37" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2040</v>
       </c>
       <c r="S37" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2041</v>
       </c>
       <c r="T37" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2042</v>
       </c>
       <c r="U37" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2043</v>
       </c>
       <c r="V37" s="13">
@@ -5772,19 +5942,19 @@
         <v>2044</v>
       </c>
       <c r="W37" s="13">
-        <f t="shared" ref="W37:Z37" si="3">V37+1</f>
+        <f t="shared" ref="W37:Z37" si="6">V37+1</f>
         <v>2045</v>
       </c>
       <c r="X37" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2046</v>
       </c>
       <c r="Y37" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2047</v>
       </c>
       <c r="Z37" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2048</v>
       </c>
       <c r="AA37" s="13">
@@ -5792,15 +5962,15 @@
         <v>2049</v>
       </c>
       <c r="AB37" s="13">
-        <f t="shared" ref="AB37" si="4">AA37+1</f>
+        <f t="shared" ref="AB37" si="7">AA37+1</f>
         <v>2050</v>
       </c>
     </row>
     <row r="38" spans="1:28">
       <c r="A38" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B38" s="21">
+        <v>127</v>
+      </c>
+      <c r="B38" s="59">
         <f t="array" ref="B38:M38">TRANSPOSE(L22:L33)</f>
         <v>5.5031947578781375E-2</v>
       </c>
@@ -5842,31 +6012,31 @@
         <v>0.55589065188784292</v>
       </c>
       <c r="O38" s="21">
-        <f t="shared" ref="O38:AB38" si="5">$M$38</f>
+        <f t="shared" ref="O38:AB38" si="8">$M$38</f>
         <v>0.55589065188784292</v>
       </c>
       <c r="P38" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.55589065188784292</v>
       </c>
       <c r="Q38" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.55589065188784292</v>
       </c>
       <c r="R38" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.55589065188784292</v>
       </c>
       <c r="S38" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.55589065188784292</v>
       </c>
       <c r="T38" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.55589065188784292</v>
       </c>
       <c r="U38" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.55589065188784292</v>
       </c>
       <c r="V38" s="21">
@@ -5874,19 +6044,19 @@
         <v>0.55589065188784292</v>
       </c>
       <c r="W38" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.55589065188784292</v>
       </c>
       <c r="X38" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.55589065188784292</v>
       </c>
       <c r="Y38" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.55589065188784292</v>
       </c>
       <c r="Z38" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.55589065188784292</v>
       </c>
       <c r="AA38" s="21">
@@ -5894,13 +6064,13 @@
         <v>0.55589065188784292</v>
       </c>
       <c r="AB38" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.55589065188784292</v>
       </c>
     </row>
     <row r="39" spans="1:28">
       <c r="A39" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B39" s="21">
         <f t="array" ref="B39:M39">TRANSPOSE(N22:N33)</f>
@@ -5944,31 +6114,31 @@
         <v>0.4</v>
       </c>
       <c r="O39" s="21">
-        <f t="shared" ref="O39:AB39" si="6">$M$39</f>
+        <f t="shared" ref="O39:AB39" si="9">$M$39</f>
         <v>0.4</v>
       </c>
       <c r="P39" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.4</v>
       </c>
       <c r="Q39" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.4</v>
       </c>
       <c r="R39" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.4</v>
       </c>
       <c r="S39" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.4</v>
       </c>
       <c r="T39" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.4</v>
       </c>
       <c r="U39" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.4</v>
       </c>
       <c r="V39" s="21">
@@ -5976,19 +6146,19 @@
         <v>0.4</v>
       </c>
       <c r="W39" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.4</v>
       </c>
       <c r="X39" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.4</v>
       </c>
       <c r="Y39" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.4</v>
       </c>
       <c r="Z39" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.4</v>
       </c>
       <c r="AA39" s="21">
@@ -5996,8 +6166,110 @@
         <v>0.4</v>
       </c>
       <c r="AB39" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28">
+      <c r="A40" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B40" s="21">
+        <f t="array" ref="B40:M40">TRANSPOSE(D22:D33)</f>
+        <v>0.09</v>
+      </c>
+      <c r="C40" s="21">
+        <v>0.11</v>
+      </c>
+      <c r="D40" s="21">
+        <v>0.13</v>
+      </c>
+      <c r="E40" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="F40" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="G40" s="21">
+        <v>0.4</v>
+      </c>
+      <c r="H40" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="I40" s="21">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J40" s="21">
+        <v>0.6</v>
+      </c>
+      <c r="K40" s="21">
+        <v>0.65</v>
+      </c>
+      <c r="L40" s="21">
+        <v>0.7</v>
+      </c>
+      <c r="M40" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="N40" s="21">
+        <f>$M$40</f>
+        <v>0.75</v>
+      </c>
+      <c r="O40" s="21">
+        <f t="shared" ref="O40:AB40" si="10">$M$40</f>
+        <v>0.75</v>
+      </c>
+      <c r="P40" s="21">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="Q40" s="21">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="R40" s="21">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="S40" s="21">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="T40" s="21">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="U40" s="21">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="V40" s="21">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="W40" s="21">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="X40" s="21">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="Y40" s="21">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="Z40" s="21">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="AA40" s="21">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="AB40" s="21">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
       </c>
     </row>
     <row r="48" spans="1:28">
@@ -6162,11 +6434,9 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AC19"/>
+  <dimension ref="A1:AD23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -6310,299 +6580,346 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="42.75">
+    <row r="17" spans="1:30" ht="42.75">
       <c r="A17" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="C17" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="D17" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="E17" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="H17" s="21">
+        <v>1</v>
+      </c>
+      <c r="I17" s="21">
+        <v>1</v>
+      </c>
+      <c r="J17" s="21">
+        <v>1</v>
+      </c>
+      <c r="K17" s="21">
+        <v>1</v>
+      </c>
+      <c r="L17" s="21">
+        <v>1</v>
+      </c>
+      <c r="M17" s="21">
+        <v>1</v>
+      </c>
+      <c r="N17" s="21">
+        <v>1</v>
+      </c>
+      <c r="O17" s="21">
+        <v>1</v>
+      </c>
+      <c r="P17" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="21">
+        <v>1</v>
+      </c>
+      <c r="R17" s="21">
+        <v>1</v>
+      </c>
+      <c r="S17" s="21">
+        <v>1</v>
+      </c>
+      <c r="T17" s="21">
+        <v>1</v>
+      </c>
+      <c r="U17" s="21">
+        <v>1</v>
+      </c>
+      <c r="V17" s="21">
+        <v>1</v>
+      </c>
+      <c r="W17" s="21">
+        <v>1</v>
+      </c>
+      <c r="X17" s="21">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="21">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="21">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="21">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="21">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" ht="28.5">
+      <c r="A18" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" s="21">
+        <v>0</v>
+      </c>
+      <c r="C18" s="21">
+        <f>'Advance Clean Trucks schedule'!B40</f>
+        <v>0.09</v>
+      </c>
+      <c r="D18" s="21">
+        <f>'Advance Clean Trucks schedule'!C40</f>
+        <v>0.11</v>
+      </c>
+      <c r="E18" s="21">
+        <f>'Advance Clean Trucks schedule'!D40</f>
+        <v>0.13</v>
+      </c>
+      <c r="F18" s="21">
+        <f>'Advance Clean Trucks schedule'!E40</f>
+        <v>0.2</v>
+      </c>
+      <c r="G18" s="21">
+        <f>'Advance Clean Trucks schedule'!F40</f>
+        <v>0.3</v>
+      </c>
+      <c r="H18" s="21">
+        <f>'Advance Clean Trucks schedule'!G40</f>
+        <v>0.4</v>
+      </c>
+      <c r="I18" s="21">
+        <f>'Advance Clean Trucks schedule'!H40</f>
+        <v>0.5</v>
+      </c>
+      <c r="J18" s="21">
+        <f>'Advance Clean Trucks schedule'!I40</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K18" s="21">
+        <f>'Advance Clean Trucks schedule'!J40</f>
+        <v>0.6</v>
+      </c>
+      <c r="L18" s="21">
+        <f>'Advance Clean Trucks schedule'!K40</f>
+        <v>0.65</v>
+      </c>
+      <c r="M18" s="21">
+        <f>'Advance Clean Trucks schedule'!L40</f>
+        <v>0.7</v>
+      </c>
+      <c r="N18" s="21">
+        <f>'Advance Clean Trucks schedule'!M40</f>
+        <v>0.75</v>
+      </c>
+      <c r="O18" s="21">
+        <f>'Advance Clean Trucks schedule'!N40</f>
+        <v>0.75</v>
+      </c>
+      <c r="P18" s="21">
+        <f>'Advance Clean Trucks schedule'!O40</f>
+        <v>0.75</v>
+      </c>
+      <c r="Q18" s="21">
+        <f>'Advance Clean Trucks schedule'!P40</f>
+        <v>0.75</v>
+      </c>
+      <c r="R18" s="21">
+        <f>'Advance Clean Trucks schedule'!Q40</f>
+        <v>0.75</v>
+      </c>
+      <c r="S18" s="21">
+        <f>'Advance Clean Trucks schedule'!R40</f>
+        <v>0.75</v>
+      </c>
+      <c r="T18" s="21">
+        <f>'Advance Clean Trucks schedule'!S40</f>
+        <v>0.75</v>
+      </c>
+      <c r="U18" s="21">
+        <f>'Advance Clean Trucks schedule'!T40</f>
+        <v>0.75</v>
+      </c>
+      <c r="V18" s="21">
+        <f>'Advance Clean Trucks schedule'!U40</f>
+        <v>0.75</v>
+      </c>
+      <c r="W18" s="21">
+        <f>'Advance Clean Trucks schedule'!V40</f>
+        <v>0.75</v>
+      </c>
+      <c r="X18" s="21">
+        <f>'Advance Clean Trucks schedule'!W40</f>
+        <v>0.75</v>
+      </c>
+      <c r="Y18" s="21">
+        <f>'Advance Clean Trucks schedule'!X40</f>
+        <v>0.75</v>
+      </c>
+      <c r="Z18" s="21">
+        <f>'Advance Clean Trucks schedule'!Y40</f>
+        <v>0.75</v>
+      </c>
+      <c r="AA18" s="21">
+        <f>'Advance Clean Trucks schedule'!Z40</f>
+        <v>0.75</v>
+      </c>
+      <c r="AB18" s="21">
+        <f>'Advance Clean Trucks schedule'!AA40</f>
+        <v>0.75</v>
+      </c>
+      <c r="AC18" s="21">
+        <f>'Advance Clean Trucks schedule'!AB40</f>
+        <v>0.75</v>
+      </c>
+      <c r="AD18" s="21"/>
+    </row>
+    <row r="20" spans="1:30" s="2" customFormat="1">
+      <c r="A20" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="2">
+        <f>EMFAC!B27</f>
+        <v>0.30619794332511285</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" s="2" customFormat="1">
+      <c r="A21" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="2">
+        <f>1-B20</f>
+        <v>0.69380205667488715</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" s="2" customFormat="1"/>
+    <row r="23" spans="1:30" ht="42.75">
+      <c r="A23" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B17" s="21">
-        <f>B18*B19</f>
-        <v>0.125</v>
-      </c>
-      <c r="C17" s="21">
-        <f t="shared" ref="C17:AC17" si="1">C18*C19</f>
-        <v>0.125</v>
-      </c>
-      <c r="D17" s="21">
+      <c r="B23" s="21">
+        <f>B17*$B$20+B18*$B$21</f>
+        <v>7.6549485831278213E-2</v>
+      </c>
+      <c r="C23" s="21">
+        <f t="shared" ref="C23:AC23" si="1">C17*$B$20+C18*$B$21</f>
+        <v>0.13899167093201806</v>
+      </c>
+      <c r="D23" s="21">
         <f t="shared" si="1"/>
-        <v>0.125</v>
-      </c>
-      <c r="E17" s="21">
+        <v>0.1528677120655158</v>
+      </c>
+      <c r="E23" s="21">
         <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-      <c r="F17" s="21">
+        <v>0.24329323903029176</v>
+      </c>
+      <c r="F23" s="21">
         <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-      <c r="G17" s="21">
+        <v>0.29185938299753389</v>
+      </c>
+      <c r="G23" s="21">
         <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-      <c r="H17" s="21">
+        <v>0.36123958866502259</v>
+      </c>
+      <c r="H23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="I17" s="21">
+        <v>0.58371876599506778</v>
+      </c>
+      <c r="I23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="J17" s="21">
+        <v>0.65309897166255637</v>
+      </c>
+      <c r="J23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="K17" s="21">
+        <v>0.68778907449630089</v>
+      </c>
+      <c r="K23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="L17" s="21">
+        <v>0.72247917733004519</v>
+      </c>
+      <c r="L23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="M17" s="21">
+        <v>0.75716928016378948</v>
+      </c>
+      <c r="M23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="N17" s="21">
+        <v>0.79185938299753378</v>
+      </c>
+      <c r="N23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="O17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="O23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="P17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="P23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="Q23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="R17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="R23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="S17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="S23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="T17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="T23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="U17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="U23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="V17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="V23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="W17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="W23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="X17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="X23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="Y17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="Y23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="Z17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="Z23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="AA17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="AA23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="AB17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="AB23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="AC17" s="21">
+        <v>0.82654948583127819</v>
+      </c>
+      <c r="AC23" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:29" ht="42.75">
-      <c r="A18" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B18" s="21">
-        <v>0.25</v>
-      </c>
-      <c r="C18" s="21">
-        <v>0.25</v>
-      </c>
-      <c r="D18" s="21">
-        <v>0.25</v>
-      </c>
-      <c r="E18" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="F18" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="G18" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="H18" s="21">
-        <v>1</v>
-      </c>
-      <c r="I18" s="21">
-        <v>1</v>
-      </c>
-      <c r="J18" s="21">
-        <v>1</v>
-      </c>
-      <c r="K18" s="21">
-        <v>1</v>
-      </c>
-      <c r="L18" s="21">
-        <v>1</v>
-      </c>
-      <c r="M18" s="21">
-        <v>1</v>
-      </c>
-      <c r="N18" s="21">
-        <v>1</v>
-      </c>
-      <c r="O18" s="21">
-        <v>1</v>
-      </c>
-      <c r="P18" s="21">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="21">
-        <v>1</v>
-      </c>
-      <c r="R18" s="21">
-        <v>1</v>
-      </c>
-      <c r="S18" s="21">
-        <v>1</v>
-      </c>
-      <c r="T18" s="21">
-        <v>1</v>
-      </c>
-      <c r="U18" s="21">
-        <v>1</v>
-      </c>
-      <c r="V18" s="21">
-        <v>1</v>
-      </c>
-      <c r="W18" s="21">
-        <v>1</v>
-      </c>
-      <c r="X18" s="21">
-        <v>1</v>
-      </c>
-      <c r="Y18" s="21">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="21">
-        <v>1</v>
-      </c>
-      <c r="AA18" s="21">
-        <v>1</v>
-      </c>
-      <c r="AB18" s="21">
-        <v>1</v>
-      </c>
-      <c r="AC18" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" ht="57">
-      <c r="A19" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="C19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="D19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="E19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="F19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="G19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="H19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="I19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="J19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="K19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="L19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="M19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="N19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="O19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="P19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="Q19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="R19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="S19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="T19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="U19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="V19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="W19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="X19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="Y19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="Z19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="AA19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="AB19" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="AC19" s="21">
-        <v>0.5</v>
+        <v>0.82654948583127819</v>
       </c>
     </row>
   </sheetData>
@@ -6612,4 +6929,265 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DE7B07-B481-4516-B55C-A623A58D07C4}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="25.796875" style="2" customWidth="1"/>
+    <col min="2" max="3" width="8.73046875" style="2"/>
+    <col min="4" max="4" width="18.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.73046875" style="2"/>
+    <col min="6" max="6" width="16.265625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.73046875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="56" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="57"/>
+      <c r="B10" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="57"/>
+      <c r="B11" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="2">
+        <v>27368</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D23" s="2">
+        <v>32274</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D24" s="2">
+        <v>26322</v>
+      </c>
+      <c r="E24" s="2">
+        <f>D24/D25</f>
+        <v>0.30619794332511285</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="2">
+        <f>D22+D23+D24</f>
+        <v>85964</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="55">
+        <f>E24</f>
+        <v>0.30619794332511285</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A9:A11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D7B09959-20CF-4C5A-A1A1-07071A8D5589}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated deeper decarb LDV EV adoption percentage and updated BPMRESP to set BAU 100 percent by 2035
</commit_message>
<xml_diff>
--- a/InputData/trans/BMRESP/BAU Min Req EV Sales Perc.xlsx
+++ b/InputData/trans/BMRESP/BAU Min Req EV Sales Perc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisB\Dropbox (Energy Innovation)\Desktop\Current CA EPS update\Revised variables\Transpo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\trans\BMRESP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A645D76-2177-4F7D-B876-E1EA40B44133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF0A2B9D-610D-4385-B008-2112D71458BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="172">
   <si>
     <t>BMRESP BAU Minimum Required EV Sales Percentage</t>
   </si>
@@ -557,17 +557,24 @@
   </si>
   <si>
     <t>Motobike-freight subscript being used for long-haul tractor trailer trucks treated equivalently to HDV-frgt.</t>
+  </si>
+  <si>
+    <t>Straightline to 2035 (ACC 2)</t>
+  </si>
+  <si>
+    <t>Post ACC2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0\ ;\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="165" formatCode="0.00_)"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -964,7 +971,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1085,6 +1092,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="105" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1687,11 +1695,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -1861,7 +1869,7 @@
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="str">
-        <f>'ZEV Waiver States'!E11</f>
+        <f>'ZEV Waiver States'!E12</f>
         <v>California, Colorado, Connecticut, Maine, Maryland, Massachusetts, New Jersey, New York, Oregon, Rhode Island, Vermont, Washington</v>
       </c>
     </row>
@@ -1899,13 +1907,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AJ58"/>
+  <dimension ref="A1:AJ59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="AJ3" sqref="E3:AJ3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:36">
       <c r="A1" t="str">
@@ -2024,416 +2035,594 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
-      <c r="A3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5">
-        <f t="shared" ref="B3:AJ3" si="0">IF(SUMIFS($B$9:$B$58,$A$9:$A$58,$A$1)=1,B5,B6)</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <f t="shared" si="0"/>
+    <row r="3" spans="1:36" s="2" customFormat="1">
+      <c r="A3" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="56">
+        <f>D6</f>
         <v>2.3355179562388431E-2</v>
       </c>
-      <c r="E3" s="5">
-        <f t="shared" si="0"/>
+      <c r="E3" s="56">
+        <f t="shared" ref="E3:G3" si="0">E6</f>
         <v>3.0832276168732849E-2</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="56">
         <f t="shared" si="0"/>
         <v>4.2396225289574353E-2</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="56">
         <f t="shared" si="0"/>
         <v>5.0699810286784948E-2</v>
       </c>
       <c r="H3" s="5">
-        <f t="shared" si="0"/>
+        <f>H5</f>
+        <v>0.118507</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" ref="I3:U3" si="1">I5</f>
+        <v>0.18631400000000001</v>
+      </c>
+      <c r="J3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.25412099999999999</v>
+      </c>
+      <c r="K3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.32192799999999999</v>
+      </c>
+      <c r="L3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.38973600000000003</v>
+      </c>
+      <c r="M3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.45754299999999998</v>
+      </c>
+      <c r="N3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.52534999999999998</v>
+      </c>
+      <c r="O3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.59315700000000005</v>
+      </c>
+      <c r="P3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.660964</v>
+      </c>
+      <c r="Q3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.72877099999999995</v>
+      </c>
+      <c r="R3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.79657900000000004</v>
+      </c>
+      <c r="S3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.86438599999999999</v>
+      </c>
+      <c r="T3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.93219300000000005</v>
+      </c>
+      <c r="U3" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="V3" s="5">
+        <f>U3</f>
+        <v>1</v>
+      </c>
+      <c r="W3" s="5">
+        <f t="shared" ref="W3:AJ3" si="2">V3</f>
+        <v>1</v>
+      </c>
+      <c r="X3" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Y3" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Z3" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AA3" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AB3" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AC3" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AD3" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AE3" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AF3" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AG3" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AH3" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AI3" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5">
+        <f>IF(SUMIFS($B$10:$B$59,$A$10:$A$59,$A$1)=1,B6,B7)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <f>IF(SUMIFS($B$10:$B$59,$A$10:$A$59,$A$1)=1,C6,C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5">
+        <f t="shared" ref="E4:AJ4" si="3">IF(SUMIFS($B$10:$B$59,$A$10:$A$59,$A$1)=1,E6,E7)</f>
+        <v>3.0832276168732849E-2</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="3"/>
+        <v>4.2396225289574353E-2</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="3"/>
+        <v>5.0699810286784948E-2</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" si="3"/>
         <v>5.6578478623361093E-2</v>
       </c>
-      <c r="I3" s="5">
-        <f t="shared" si="0"/>
+      <c r="I4" s="5">
+        <f t="shared" si="3"/>
         <v>6.3298146163166397E-2</v>
       </c>
-      <c r="J3" s="5">
-        <f t="shared" si="0"/>
+      <c r="J4" s="5">
+        <f t="shared" si="3"/>
         <v>6.9598265212907795E-2</v>
       </c>
-      <c r="K3" s="5">
-        <f t="shared" si="0"/>
+      <c r="K4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="L3" s="5">
-        <f t="shared" si="0"/>
+      <c r="L4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="M3" s="5">
-        <f t="shared" si="0"/>
+      <c r="M4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="N3" s="5">
-        <f t="shared" si="0"/>
+      <c r="N4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="O3" s="5">
-        <f t="shared" si="0"/>
+      <c r="O4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="P3" s="5">
-        <f t="shared" si="0"/>
+      <c r="P4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="Q3" s="5">
-        <f t="shared" si="0"/>
+      <c r="Q4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="R3" s="5">
-        <f t="shared" si="0"/>
+      <c r="R4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="S3" s="5">
-        <f t="shared" si="0"/>
+      <c r="S4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="T3" s="5">
-        <f t="shared" si="0"/>
+      <c r="T4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="U3" s="5">
-        <f t="shared" si="0"/>
+      <c r="U4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="V3" s="5">
-        <f t="shared" si="0"/>
+      <c r="V4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="W3" s="5">
-        <f t="shared" si="0"/>
+      <c r="W4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="X3" s="5">
-        <f t="shared" si="0"/>
+      <c r="X4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="Y3" s="5">
-        <f t="shared" si="0"/>
+      <c r="Y4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="Z3" s="5">
-        <f t="shared" si="0"/>
+      <c r="Z4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="AA3" s="5">
-        <f t="shared" si="0"/>
+      <c r="AA4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="AB3" s="5">
-        <f t="shared" si="0"/>
+      <c r="AB4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="AC3" s="5">
-        <f t="shared" si="0"/>
+      <c r="AC4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="AD3" s="5">
-        <f t="shared" si="0"/>
+      <c r="AD4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="AE3" s="5">
-        <f t="shared" si="0"/>
+      <c r="AE4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="AF3" s="5">
-        <f t="shared" si="0"/>
+      <c r="AF4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="AG3" s="5">
-        <f t="shared" si="0"/>
+      <c r="AG4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="AH3" s="5">
-        <f t="shared" si="0"/>
+      <c r="AH4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="AI3" s="5">
-        <f t="shared" si="0"/>
+      <c r="AI4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
-      <c r="AJ3" s="5">
-        <f t="shared" si="0"/>
+      <c r="AJ4" s="5">
+        <f t="shared" si="3"/>
         <v>7.5536124138948738E-2</v>
       </c>
     </row>
     <row r="5" spans="1:36">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>2.3355179562388431E-2</v>
-      </c>
-      <c r="E5">
-        <v>3.0832276168732849E-2</v>
-      </c>
-      <c r="F5">
-        <v>4.2396225289574353E-2</v>
-      </c>
-      <c r="G5">
-        <v>5.0699810286784948E-2</v>
+      <c r="A5" t="s">
+        <v>170</v>
       </c>
       <c r="H5">
-        <v>5.6578478623361093E-2</v>
+        <v>0.118507</v>
       </c>
       <c r="I5">
-        <v>6.3298146163166397E-2</v>
+        <v>0.18631400000000001</v>
       </c>
       <c r="J5">
-        <v>6.9598265212907795E-2</v>
+        <v>0.25412099999999999</v>
       </c>
       <c r="K5">
-        <v>7.5536124138948738E-2</v>
+        <v>0.32192799999999999</v>
       </c>
       <c r="L5">
-        <v>7.5536124138948738E-2</v>
+        <v>0.38973600000000003</v>
       </c>
       <c r="M5">
-        <v>7.5536124138948738E-2</v>
+        <v>0.45754299999999998</v>
       </c>
       <c r="N5">
-        <v>7.5536124138948738E-2</v>
+        <v>0.52534999999999998</v>
       </c>
       <c r="O5">
-        <v>7.5536124138948738E-2</v>
+        <v>0.59315700000000005</v>
       </c>
       <c r="P5">
-        <v>7.5536124138948738E-2</v>
+        <v>0.660964</v>
       </c>
       <c r="Q5">
-        <v>7.5536124138948738E-2</v>
+        <v>0.72877099999999995</v>
       </c>
       <c r="R5">
-        <v>7.5536124138948738E-2</v>
+        <v>0.79657900000000004</v>
       </c>
       <c r="S5">
-        <v>7.5536124138948738E-2</v>
+        <v>0.86438599999999999</v>
       </c>
       <c r="T5">
-        <v>7.5536124138948738E-2</v>
+        <v>0.93219300000000005</v>
       </c>
       <c r="U5">
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="V5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="W5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="X5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="Y5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="Z5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="AA5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="AB5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="AC5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="AD5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="AE5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="AF5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="AG5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="AH5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="AI5">
-        <v>7.5536124138948738E-2</v>
-      </c>
-      <c r="AJ5">
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:36">
       <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2.3355179562388431E-2</v>
+      </c>
+      <c r="E6">
+        <v>3.0832276168732849E-2</v>
+      </c>
+      <c r="F6">
+        <v>4.2396225289574353E-2</v>
+      </c>
+      <c r="G6">
+        <v>5.0699810286784948E-2</v>
+      </c>
+      <c r="H6">
+        <v>5.6578478623361093E-2</v>
+      </c>
+      <c r="I6">
+        <v>6.3298146163166397E-2</v>
+      </c>
+      <c r="J6">
+        <v>6.9598265212907795E-2</v>
+      </c>
+      <c r="K6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="L6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="M6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="N6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="O6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="P6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="Q6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="R6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="S6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="T6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="U6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="V6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="W6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="X6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="Y6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="Z6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="AA6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="AB6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="AC6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="AD6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="AE6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="AF6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="AG6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="AH6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="AI6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+      <c r="AJ6">
+        <v>7.5536124138948738E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6">
-        <v>0</v>
-      </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
-      <c r="AG6">
-        <v>0</v>
-      </c>
-      <c r="AH6">
-        <v>0</v>
-      </c>
-      <c r="AI6">
-        <v>0</v>
-      </c>
-      <c r="AJ6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:36">
-      <c r="A8" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36">
-      <c r="A9" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:36">
       <c r="A10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:36">
       <c r="A11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>100</v>
+        <v>20</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:36">
       <c r="A12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:36">
       <c r="A13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:36">
       <c r="A14" s="4" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2441,7 +2630,7 @@
     </row>
     <row r="15" spans="1:36">
       <c r="A15" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2449,70 +2638,70 @@
     </row>
     <row r="16" spans="1:36">
       <c r="A16" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2520,7 +2709,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2528,164 +2717,172 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53">
-        <v>1</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="4" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2701,13 +2898,13 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T21" sqref="R21:T22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -2822,16 +3019,16 @@
         <v>69</v>
       </c>
       <c r="B2">
-        <f>'ZEV Waiver States'!B3</f>
+        <f>'ZEV Waiver States'!B4</f>
         <v>0</v>
       </c>
       <c r="C2">
-        <f>'ZEV Waiver States'!C3</f>
+        <f>'ZEV Waiver States'!C4</f>
         <v>0</v>
       </c>
       <c r="D2">
-        <f>'ZEV Waiver States'!D3</f>
-        <v>2.3355179562388431E-2</v>
+        <f>'ZEV Waiver States'!D4</f>
+        <v>0</v>
       </c>
       <c r="E2">
         <f>'ZEV Waiver States'!E3</f>
@@ -2847,119 +3044,119 @@
       </c>
       <c r="H2">
         <f>'ZEV Waiver States'!H3</f>
-        <v>5.6578478623361093E-2</v>
+        <v>0.118507</v>
       </c>
       <c r="I2">
         <f>'ZEV Waiver States'!I3</f>
-        <v>6.3298146163166397E-2</v>
+        <v>0.18631400000000001</v>
       </c>
       <c r="J2">
         <f>'ZEV Waiver States'!J3</f>
-        <v>6.9598265212907795E-2</v>
+        <v>0.25412099999999999</v>
       </c>
       <c r="K2">
         <f>'ZEV Waiver States'!K3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>0.32192799999999999</v>
       </c>
       <c r="L2">
         <f>'ZEV Waiver States'!L3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>0.38973600000000003</v>
       </c>
       <c r="M2">
         <f>'ZEV Waiver States'!M3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>0.45754299999999998</v>
       </c>
       <c r="N2">
         <f>'ZEV Waiver States'!N3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>0.52534999999999998</v>
       </c>
       <c r="O2">
         <f>'ZEV Waiver States'!O3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>0.59315700000000005</v>
       </c>
       <c r="P2">
         <f>'ZEV Waiver States'!P3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>0.660964</v>
       </c>
       <c r="Q2">
         <f>'ZEV Waiver States'!Q3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>0.72877099999999995</v>
       </c>
       <c r="R2">
         <f>'ZEV Waiver States'!R3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>0.79657900000000004</v>
       </c>
       <c r="S2">
         <f>'ZEV Waiver States'!S3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>0.86438599999999999</v>
       </c>
       <c r="T2">
         <f>'ZEV Waiver States'!T3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>0.93219300000000005</v>
       </c>
       <c r="U2">
         <f>'ZEV Waiver States'!U3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="V2">
         <f>'ZEV Waiver States'!V3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="W2">
         <f>'ZEV Waiver States'!W3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="X2">
         <f>'ZEV Waiver States'!X3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="Y2">
         <f>'ZEV Waiver States'!Y3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="Z2">
         <f>'ZEV Waiver States'!Z3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="AA2">
         <f>'ZEV Waiver States'!AA3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="AB2">
         <f>'ZEV Waiver States'!AB3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="AC2">
         <f>'ZEV Waiver States'!AC3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="AD2">
         <f>'ZEV Waiver States'!AD3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="AE2">
         <f>'ZEV Waiver States'!AE3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="AF2">
         <f>'ZEV Waiver States'!AF3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="AG2">
         <f>'ZEV Waiver States'!AG3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="AH2">
         <f>'ZEV Waiver States'!AH3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="AI2">
         <f>'ZEV Waiver States'!AI3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
       <c r="AJ2">
         <f>'ZEV Waiver States'!AJ3</f>
-        <v>7.5536124138948738E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -3556,9 +3753,9 @@
       <selection activeCell="DV22" sqref="DV22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -4423,19 +4620,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="2"/>
-    <col min="2" max="2" width="16.81640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="2"/>
-    <col min="5" max="5" width="8.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="8.7265625" style="2"/>
-    <col min="14" max="14" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="8.7109375" style="2"/>
+    <col min="2" max="2" width="16.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="2"/>
+    <col min="5" max="5" width="8.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="8.7109375" style="2"/>
+    <col min="14" max="14" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -4474,20 +4671,20 @@
       <c r="H17" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="J17" s="56" t="s">
+      <c r="J17" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="57"/>
-      <c r="N17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="59"/>
       <c r="O17" s="12"/>
-      <c r="P17" s="56" t="s">
+      <c r="P17" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="Q17" s="57"/>
-      <c r="R17" s="57"/>
-      <c r="S17" s="58"/>
+      <c r="Q17" s="58"/>
+      <c r="R17" s="58"/>
+      <c r="S17" s="59"/>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="13">
@@ -5119,20 +5316,20 @@
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="2"/>
-    <col min="2" max="2" width="12.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.08984375" style="2"/>
-    <col min="5" max="5" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.08984375" style="2"/>
-    <col min="10" max="11" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.08984375" style="2"/>
-    <col min="16" max="16" width="9.81640625" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="9.08984375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="12.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="2"/>
+    <col min="10" max="11" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="2"/>
+    <col min="16" max="16" width="9.85546875" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -5146,25 +5343,25 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="56" t="s">
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="56" t="s">
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="M20" s="57"/>
-      <c r="N20" s="58"/>
+      <c r="M20" s="58"/>
+      <c r="N20" s="59"/>
     </row>
     <row r="21" spans="1:14">
       <c r="B21" s="42" t="s">
@@ -6450,9 +6647,9 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6592,7 +6789,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="43.5">
+    <row r="17" spans="1:30" ht="45">
       <c r="A17" s="8" t="s">
         <v>119</v>
       </c>
@@ -6681,7 +6878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="29">
+    <row r="18" spans="1:30" ht="30">
       <c r="A18" s="8" t="s">
         <v>166</v>
       </c>
@@ -6817,7 +7014,7 @@
       </c>
     </row>
     <row r="22" spans="1:30" s="2" customFormat="1"/>
-    <row r="23" spans="1:30" ht="43.5">
+    <row r="23" spans="1:30" ht="45">
       <c r="A23" s="8" t="s">
         <v>118</v>
       </c>
@@ -6954,14 +7151,14 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="8.7265625" style="2"/>
-    <col min="4" max="4" width="18.36328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="2"/>
-    <col min="6" max="6" width="16.26953125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="25.85546875" style="2" customWidth="1"/>
+    <col min="2" max="3" width="8.7109375" style="2"/>
+    <col min="4" max="4" width="18.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="2"/>
+    <col min="6" max="6" width="16.28515625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -7014,7 +7211,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="60" t="s">
         <v>144</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -7022,13 +7219,13 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="59"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="2" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="59"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="2" t="s">
         <v>155</v>
       </c>

</xml_diff>